<commit_message>
Test excel Filled Out
</commit_message>
<xml_diff>
--- a/projekt_planungPräsi/Tests.xlsx
+++ b/projekt_planungPräsi/Tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timci\OneDrive - TBZ\Desktop\blj2025-uek216-uek-team-1-wc\projekt_planungPräsi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A412B1C9-7A91-4F70-A49F-20AA7E6F9149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BCB0A3E-6E2C-47FA-A9AC-01A84A747F0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Tests</t>
   </si>
@@ -72,7 +72,22 @@
     <t>keine verbesserungen</t>
   </si>
   <si>
-    <t xml:space="preserve">Timer </t>
+    <t>Timer coutdown getestet und mit sensor angesteuert</t>
+  </si>
+  <si>
+    <t>countdown läuft türe detection optimierbar</t>
+  </si>
+  <si>
+    <t>Distantce logik verbessern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">time 0 alarm </t>
+  </si>
+  <si>
+    <t>Alarm wird ausgelöst</t>
+  </si>
+  <si>
+    <t>sensor Türe Test logik verbesserungen</t>
   </si>
 </sst>
 </file>
@@ -393,7 +408,7 @@
   <dimension ref="A1:F78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -458,6 +473,12 @@
       <c r="D3" t="s">
         <v>9</v>
       </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
@@ -466,8 +487,17 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
       <c r="D4" t="s">
         <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -475,7 +505,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -486,7 +516,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -495,6 +525,12 @@
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>